<commit_message>
Updated InDesign file. Add E000 for OpenType bogus glyph.
</commit_message>
<xml_diff>
--- a/source/glyph_data.xlsx
+++ b/source/glyph_data.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="801">
   <si>
     <t>USV</t>
   </si>
@@ -2404,6 +2404,48 @@
   </si>
   <si>
     <t>uni02D0</t>
+  </si>
+  <si>
+    <t>uni1C191C37</t>
+  </si>
+  <si>
+    <t>uni1C1B1C37</t>
+  </si>
+  <si>
+    <t>uni1C001C371C25</t>
+  </si>
+  <si>
+    <t>uni1C031C371C25</t>
+  </si>
+  <si>
+    <t>uni1C1D1C371C25</t>
+  </si>
+  <si>
+    <t>uni1C101C37</t>
+  </si>
+  <si>
+    <t>uni1C211C37</t>
+  </si>
+  <si>
+    <t>uni1C001C371C24</t>
+  </si>
+  <si>
+    <t>uni1C001C371C251C24</t>
+  </si>
+  <si>
+    <t>uni1C031C371C24</t>
+  </si>
+  <si>
+    <t>uni1C131C371C25</t>
+  </si>
+  <si>
+    <t>uni1C1D1C371C24</t>
+  </si>
+  <si>
+    <t>uni1C1D1C371C251C24</t>
+  </si>
+  <si>
+    <t>uniE000</t>
   </si>
 </sst>
 </file>
@@ -2747,10 +2789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E432"/>
+  <dimension ref="A1:E446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7394,6 +7436,118 @@
         <v>453</v>
       </c>
     </row>
+    <row r="433" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C433" t="s">
+        <v>787</v>
+      </c>
+      <c r="D433" s="2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="434" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C434" t="s">
+        <v>788</v>
+      </c>
+      <c r="D434" s="2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="435" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C435" t="s">
+        <v>789</v>
+      </c>
+      <c r="D435" s="2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="436" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C436" t="s">
+        <v>790</v>
+      </c>
+      <c r="D436" s="2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="437" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C437" t="s">
+        <v>791</v>
+      </c>
+      <c r="D437" s="2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="438" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C438" t="s">
+        <v>792</v>
+      </c>
+      <c r="D438" s="2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="439" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C439" t="s">
+        <v>793</v>
+      </c>
+      <c r="D439" s="2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="440" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C440" t="s">
+        <v>794</v>
+      </c>
+      <c r="D440" s="2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="441" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C441" t="s">
+        <v>795</v>
+      </c>
+      <c r="D441" s="2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="442" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C442" t="s">
+        <v>796</v>
+      </c>
+      <c r="D442" s="2">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="443" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C443" t="s">
+        <v>797</v>
+      </c>
+      <c r="D443" s="2">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="444" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C444" t="s">
+        <v>798</v>
+      </c>
+      <c r="D444" s="2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="445" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C445" t="s">
+        <v>799</v>
+      </c>
+      <c r="D445" s="2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="446" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C446" t="s">
+        <v>800</v>
+      </c>
+      <c r="D446" s="2">
+        <v>467</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E432">
     <sortCondition ref="D2:D432"/>

</xml_diff>